<commit_message>
ndimas add menu prov
</commit_message>
<xml_diff>
--- a/assets/data/menu.xlsx
+++ b/assets/data/menu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mikroskil\Sem4\Visual Studio Code\ProjectNew\flutter_application_1\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E345BC-05FF-44AF-A8DC-68EAB10EAB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B241A590-23C6-4806-B1D0-D542A00DD259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7056" yWindow="156" windowWidth="16332" windowHeight="11496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="123">
   <si>
     <t>A01</t>
   </si>
@@ -174,15 +174,9 @@
     <t>Melon Soda</t>
   </si>
   <si>
-    <t>Cheese Cake</t>
-  </si>
-  <si>
     <t>Special Pudding</t>
   </si>
   <si>
-    <t>Curry bun, also known as kare pan or curry puff, a popular Japanese snack or street food item. It consists of a soft and fluffy bread bun filled with a rich and flavorful curry filling. The curry filling is typically made with a combination of ingredients such as potatoes, carrots, onions, and meat (often minced beef or pork), all cooked in a fragrant blend of spices and curry powder. The bread bun that encases the curry filling is usually made from a slightly sweet and fluffy dough, providing a pleasant contrast to the savory curry inside. The bun is often deep-fried to achieve a crispy outer layer.</t>
-  </si>
-  <si>
     <t>Croquettes are a popular dish made from a mixture of ingredients such as mashed potatoes, vegetables, meat, fish, or cheese. The ingredients are typically combined, seasoned, and shaped into small cylindrical or rounded shapes, similar to small logs or balls. The croquette mixture is then coated in breadcrumbs and fried until crispy and golden brown. Can be enjoyed on their own or accompanied by dipping sauces, such as aioli, ketchup, or mustard.</t>
   </si>
   <si>
@@ -205,6 +199,204 @@
   </si>
   <si>
     <t>Popular and delicious seafood dish that features succulent shrimp coated in a crispy, golden-brown crust. Coated in a seasoned batter or breading to add flavor and create a crispy texture. The batter or breading can be made from a variety of ingredients, including flour, cornmeal, breadcrumbs, or a combination of these, along with spices, herbs, and seasonings to enhance the taste.</t>
+  </si>
+  <si>
+    <t>Delicious soup cooked with pork meat or bones, vegetables, herbs and spices. The pork usually simmered for a long time to extract its rich flavors and create a hearty broth. Various cuts of pork can be used in pork soup such as pork ribs, shoulder or belly. Additionally, pork bones, such as ham hocks or trotters. Another ingredients such as carrots, onions, celery, potatoes, mushrooms, corn, peas, or beans.</t>
+  </si>
+  <si>
+    <t>Sandwiches are a popular dish made from two slices of bread with a filling in between. The filling such as meats, cheese, vegetables, spreds and sauces, condiments, egg, tuna or chicken salad. Sandwiches are not only conveniet but also ofer a balanced combination of carbohydrates, proteins, and vegetables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delicious and nutritious vegetarian or vegan dish that showcases tofu as the main ingredient.To prepare tofu steak, the tofu block is typically sliced into thick slabs or cutlets to resemble the shape of a traditional steak. The tofu slices are then marinated to infuse them with flavor and enhance their taste. Common marinades for tofu steak include soy sauce, garlic, ginger, sesame oil, and various herbs and spices.
+</t>
+  </si>
+  <si>
+    <t>Steam Potatoes are made from sweet potato seasoned with a sprinkle salt and pepper or herbs like parsley or dill.Steaming potatoes helps to retain their natural flavors and nutrients, making them a nutritious and versatile addition to your meals. They are low in fat, cholesterol-free, and a good source of dietary fiber, potassium, and vitamin C.</t>
+  </si>
+  <si>
+    <t>Delicious tender pieces of beef cooked slowly with vegetables, herbs, and flavorful broth.</t>
+  </si>
+  <si>
+    <t>Beef stew is a hearty and comforting dish that features tender pieces of beef cooked slowly with vegetables, herbs, and flavorful broth. It is a classic dish that is loved for its rich and savory flavors.Beef stew is best enjoyed hot, straight from the pot.The slow cooking process results in tender beef that is infused with the rich flavors of the broth and vegetables.</t>
+  </si>
+  <si>
+    <t>Delicious tender slices of pork belly cooked in a rich and flavorful braising sauce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Braised pork belly, also known as Dongpo pork or hong shao rou, is a classic Chinese dish that features succulent and tender slices of pork belly cooked in a rich and flavorful braising sauce. It is a popular dish known for its melt-in-your-mouth texture and savory taste.Braised pork belly is often enjoyed with steamed rice or served as a filling for steamed buns. 
+</t>
+  </si>
+  <si>
+    <t>Carpaccio is a popular Italian dish that consists of thinly sliced raw meat or fish, typically beef or seafood.Carpaccio showcases the natural flavors and textures of the raw meat or fish, allowing you to savor its tenderness and subtle taste. The combination of the delicate slices, the richness of the olive oil, and the seasoning creates a delightful culinary experience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curry Rice is a popular dish that originated in Japan but draws inspiration from Indian cuisine. It consists of a flavorful curry sauce served over steamed rice, creating a hearty and satisfying meal.With its combination of fragrant spices, tender meat, flavorful vegetables, and fluffy rice, Curry Rice offers a comforting and satisfying dining experience. </t>
+  </si>
+  <si>
+    <t>Ground meat patty seasoned with breadcrumbs, onions, garlic, eggs, salt, and  pepper</t>
+  </si>
+  <si>
+    <t>Delicious ground meat patty, egg, vegetables, and sauce placed between two slices of a soft bun</t>
+  </si>
+  <si>
+    <t>deep-fried pork cutlet served over a bowl of steamed rice and topped with a savory sauce and beaten eggs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crepes are thin, delicate pancakes filled with a variety of delicious ingredients such as fresh fruits, chocolate spread, whipped cream, or jam. Crepes are known for their delicate texture and subtle flavor, allowing the fillings and toppings to shine. They can be enjoyed warm or at room temperature, and their versatility makes them suitable for any time of the day.
+</t>
+  </si>
+  <si>
+    <t>Thin crepes-pancake filled with fresh fruits, chocolate spread, whipped cream, or jam</t>
+  </si>
+  <si>
+    <t>Delicious soup with pork meat and bones,with additional vegetables, herbs and spices.</t>
+  </si>
+  <si>
+    <t>Two slices of garlicky-bread with meat-fillin and vegetables in between</t>
+  </si>
+  <si>
+    <t>Delicious vegetarian dish with combination of grilled-tofu with soy sauce, garlic, and various herbs and spices</t>
+  </si>
+  <si>
+    <t>Delicious steamed potato seasoned with a sprinkle salt and pepper and various spices</t>
+  </si>
+  <si>
+    <t>Enjoy your morning routine with homemade beacon slices, egg, salad and butter-bread</t>
+  </si>
+  <si>
+    <t>spaghetti with addition thinly sliced raw meat or fish seasoned with olive oil</t>
+  </si>
+  <si>
+    <t>Delicious traditional Japannese curry sauce and vagetables served with steamed rice</t>
+  </si>
+  <si>
+    <t>Popular Italian pasta with traditional sauce combines with japannese sticky natto</t>
+  </si>
+  <si>
+    <t>Popular Japanese snack or street food item. It consists of a soft and fluffy bread bun filled with a rich and flavorful curry filling. The filling is typically made with a combination of ingredients such as potatoes, carrots, onions, and meat (often minced beef or pork), all cooked in a fragrant blend of spices and curry powder. The bread bun that encases the curry filling is usually made from a slightly sweet and fluffy dough, providing a pleasant contrast to the savory curry inside. The bun is often deep-fried to achieve a crispy outer layer.</t>
+  </si>
+  <si>
+    <t>Enjoyful morning routine with 'Breakfast Special' ala American-British style, with homemade served beacon slices sizzled with olive oil and seasoning to perfection ala Randumu seasoning, typical morning pan-egg with sweet touch of mustard and mayonise, moring salad start with healty fruits and vegetables served with mayonise and sour cream and toasted butter spread bread to start your day, sip it with our favorite morning coffee to fulfil your day with happiness, colorful and joy.</t>
+  </si>
+  <si>
+    <t>Hamburg Steak is a popular dish made with a combination of ground beef and pork that are grind into one plain meat, seasoned with various ingredients, herbs and spices to add such seasoning, herbs and spices and such more as breadcrumbs, onions, garlic, eggs, and various seasonings like salt, pepper, and Worcestershire sauce, that with sweet salty tase and umami in your taste buds. These menu is popular in heavy steak menu, with also loads of blackpaper and barberque sauce available at Randumu</t>
+  </si>
+  <si>
+    <t>Hamburgers are highly customizable, allowing individuals to personalize their burgers with a wide variety of toppings and condiments. Some popular toppings include lettuce, tomato, onion, pickles, cheese, bacon, and sautéed mushrooms.Hamburgers are often served with a side of French fries, onion rings, or a salad. You can also order here with your personalized additions toppings with also additions sauce to extends its variety to your likings.</t>
+  </si>
+  <si>
+    <t>assets/food/Curry_bun.png</t>
+  </si>
+  <si>
+    <t>assets/food/Fried_seafood.png</t>
+  </si>
+  <si>
+    <t>assets/food/Fried_shrimp.png</t>
+  </si>
+  <si>
+    <t>assets/food/Pork_soup.png</t>
+  </si>
+  <si>
+    <t>assets/food/Sandwich.png</t>
+  </si>
+  <si>
+    <t>assets/food/Tofu_steak.png</t>
+  </si>
+  <si>
+    <t>assets/food/Steam_potato.png</t>
+  </si>
+  <si>
+    <t>assets/food/Beef_stew.png</t>
+  </si>
+  <si>
+    <t>assets/food/Braised_pork.png</t>
+  </si>
+  <si>
+    <t>assets/food/Breakfast_special.png</t>
+  </si>
+  <si>
+    <t>assets/food/Carpaccio.png</t>
+  </si>
+  <si>
+    <t>assets/food/Curry_rice.png</t>
+  </si>
+  <si>
+    <t>assets/food/Hamburg_steak.png</t>
+  </si>
+  <si>
+    <t>assets/food/Hamburger.png</t>
+  </si>
+  <si>
+    <t>assets/food/Katsudon.png</t>
+  </si>
+  <si>
+    <t>assets/food/Natto_spaghetti.png</t>
+  </si>
+  <si>
+    <t>Katsudon is a popular Japanese dish that features a breaded and deep-fried pork cutlet, known as tonkatsu, served on a bed of rice and topped with a flavorful egg and onion mixture. A sweet and savory sauce is prepared by combining ingredients such as soy sauce, mirin (a sweet rice wine), sugar, and dashi (a Japanese soup stock). Sliced onions are sautéed until they become translucent and tender, and then the sauce is poured over the onions to create a flavorful mixture.</t>
+  </si>
+  <si>
+    <t>Natto spaghetti is a unique and flavorful dish that combines traditional Italian pasta with a popular Japanese ingredient called natto. Natto is prepared by mixing it with a sauce made from soy sauce, mustard, and sometimes a bit of sugar or honey. Natto, known for its pungent smell and sticky texture, is made by fermenting soybeans with a specific strain of bacteria. It has a unique, savory, and slightly nutty taste that is an acquired taste for some, but beloved by many in Japanese cuisine.</t>
+  </si>
+  <si>
+    <t>a classic and versatile dish made from beaten eggs cooked in a frying pan or skillet. It is a popular breakfast or brunch option in many cultures around the world, valued for its simplicity, quick preparation, and ability to incorporate a variety of fillings. Common fillings include grated or diced cheese, cooked vegetables such as onions, bell peppers, mushrooms, spinach, or tomatoes, and cooked meats like ham, bacon, or sausage. Herbs, spices, and seasonings can also be added to enhance the flavor profile.</t>
+  </si>
+  <si>
+    <t>Classic and versatile dish made from beaten eggs cooked in a frying pan or skillet. Cooked with cheese, vegetables, meats and spices</t>
+  </si>
+  <si>
+    <t>Assorted cookies refer to a collection or assortment of different types of cookies that are packaged or served together. These cookies come in a variety of shapes, sizes, flavors, and textures, offering a delightful assortment of sweet treats for cookie lovers. Varieties such as chocolate chip cookies, oatmeal cookies, sugar cookies, peanut butter cookies, shortbread cookies, gingerbread cookies, snickerdoodles, and more. The assortment may also feature cookies with various fillings, toppings, or mix-ins such as nuts, dried fruits, or chocolate chunks.</t>
+  </si>
+  <si>
+    <t>Collection or assortment of different types of cookies in a variety of shapes, flavors, and textures. A delightful assortment of sweet treats for cookie lovers.</t>
+  </si>
+  <si>
+    <t>A decadent and indulgent dessert that combines layers of rich chocolate components to create a visually appealing and delicious treat. Consists of a combination of chocolate mousse or pudding, whipped cream, chocolate sauce, and various toppings. The base of a chocolate parfait is often a creamy and smooth chocolate mousse or pudding. This layer provides a luscious and velvety texture that melts in the mouth, delivering a rich chocolate flavor. The mousse or pudding is usually made from high-quality chocolate, eggs, sugar, and cream.</t>
+  </si>
+  <si>
+    <t>A decadent and indulgent dessert that combines layers of rich chocolate components to create a visually appealing and delicious treat</t>
+  </si>
+  <si>
+    <t>A refreshing and vibrant carbonated beverage that is popular in Japan and other parts of the world. It is known for its distinct melon flavor and bright green color, which gives it a unique and appealing appearance. It has a sweet and fruity taste that resembles the flavor of ripe melons, such as honeydew or cantaloupe. The soda is usually made by combining carbonated water with melon-flavored syrup or extract. The bright green color of melon soda adds to its visual appeal and is often associated with its refreshing and fun nature.</t>
+  </si>
+  <si>
+    <t>A refreshing and vibrant carbonated beverage with distinct melon flavor and bright green color and fruity taste</t>
+  </si>
+  <si>
+    <t>Caramel egg pudding, also known as caramel custard or flan, is a luscious and creamy dessert with a silky smooth texture. Caramel egg pudding consists of a rich custard base made from a mixture of eggs, milk or cream, sugar, and vanilla extract. The custard is gently cooked and then cooled to set, resulting in a smooth and jiggly texture. The defining feature of caramel egg pudding is the layer of golden caramel sauce that lines the bottom of the dessert. With special also add-ons fruit and cream taste.</t>
+  </si>
+  <si>
+    <t>Luscious and creamy dessert with a silky smooth texture, rich custard base from mixture of eggs, cream, sugar, and vanilla extract</t>
+  </si>
+  <si>
+    <t>A delicate and fluffy dessert that originates from Japan. It is a unique variation of the traditional cheesecake. Made by using a few basic ingredients, including cream cheese, eggs, sugar, and flour. The cream cheese is typically softened and mixed with sugar until smooth and creamy. Egg yolks are added to the mixture, followed by a small amount of flour to stabilize the batter. The egg whites are separately whipped into a meringue with sugar until stiff peaks form. The meringue is then gently folded into the cream cheese mixture, creating a light and airy batter.</t>
+  </si>
+  <si>
+    <t>A delicate and fluffy dessert with unique Japan taste from traditional cheesecake,  light and airy texture.</t>
+  </si>
+  <si>
+    <t>assets/food/Omelette.png</t>
+  </si>
+  <si>
+    <t>assets/food/Assorted_cookies.png</t>
+  </si>
+  <si>
+    <t>assets/food/Chocolate_parfait.png</t>
+  </si>
+  <si>
+    <t>assets/food/Crepes.png</t>
+  </si>
+  <si>
+    <t>assets/food/Melon_soda.png</t>
+  </si>
+  <si>
+    <t>assets/food/Pudding.png</t>
+  </si>
+  <si>
+    <t>assets/food/Souffle.png</t>
+  </si>
+  <si>
+    <t>Souffle Cheese Cake</t>
   </si>
 </sst>
 </file>
@@ -255,13 +447,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,400 +737,573 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="91.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="G1" s="2">
         <v>45000</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="2">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="2">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="F6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="2">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="2">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="2">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="2">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="2">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="2">
+        <v>45500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="2">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="D13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="2">
+        <v>53000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="D14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="2">
+        <v>67000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="D15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="2">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="D16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="2">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="D17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="2">
+        <v>65500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="D18" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" s="2">
+        <v>43500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="D19" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="D20" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="2">
+        <v>43500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="D21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="2">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="D22" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" s="2">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="C23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="2">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="2"/>
+      <c r="C24" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G24" s="2">
+        <v>47500</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>